<commit_message>
Excel with calculations-testing update.
</commit_message>
<xml_diff>
--- a/docs/Obliczenia2.xlsx
+++ b/docs/Obliczenia2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>Wielkość alkoholu</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t>2 / 1 / 0,5</t>
+  </si>
+  <si>
+    <t>Odwrócenie wzoru:</t>
+  </si>
+  <si>
+    <t>PromCH = TOTAL - ELI * h</t>
+  </si>
+  <si>
+    <t>0=TOTAL-ELI*h</t>
+  </si>
+  <si>
+    <t>TOTAL = ELI * h</t>
+  </si>
+  <si>
+    <t>h = TOTAL / ELI</t>
   </si>
 </sst>
 </file>
@@ -11095,7 +11110,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11210,6 +11225,9 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -11219,6 +11237,9 @@
         <f>$B$12-$G$6*A14</f>
         <v>0.93492954220016233</v>
       </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -11228,6 +11249,9 @@
         <f t="shared" ref="B15:B27" si="0">$B$12-$G$6*A15</f>
         <v>0.81492954220016234</v>
       </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -11237,8 +11261,11 @@
         <f t="shared" si="0"/>
         <v>0.69492954220016234</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -11246,8 +11273,11 @@
         <f t="shared" si="0"/>
         <v>0.57492954220016235</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -11256,7 +11286,7 @@
         <v>0.45492954220016235</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -11265,7 +11295,7 @@
         <v>0.33492954220016236</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
@@ -11274,7 +11304,7 @@
         <v>0.21492954220016236</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>8</v>
       </c>
@@ -11283,7 +11313,7 @@
         <v>9.4929542200162365E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
@@ -11292,7 +11322,7 @@
         <v>-2.5070457799837742E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10</v>
       </c>
@@ -11301,7 +11331,7 @@
         <v>-0.14507045779983763</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>11</v>
       </c>
@@ -11310,7 +11340,7 @@
         <v>-0.26507045779983751</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -11319,7 +11349,7 @@
         <v>-0.38507045779983762</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>13</v>
       </c>
@@ -11328,7 +11358,7 @@
         <v>-0.50507045779983772</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>14</v>
       </c>

</xml_diff>